<commit_message>
update feature external resps
</commit_message>
<xml_diff>
--- a/media/EJMNzZUoC4261SiH4LPKhjASoF6VQzjJT6y1mk5WIlk82XxFYZophZdi2021_11_29_15_22_55_471395.xlsx
+++ b/media/EJMNzZUoC4261SiH4LPKhjASoF6VQzjJT6y1mk5WIlk82XxFYZophZdi2021_11_29_15_22_55_471395.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mohit Satija</t>
+          <t>mohit</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,37 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>kuch bhi</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>mohit@gmail.com</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>piyush kumar</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>bollyknow@gmail.com</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>